<commit_message>
Guión corregido editor Solicitud Gráfica CN_07_08_CO
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado07/guion08/Escaleta CN_07_08_CO.xlsx
+++ b/fuentes/contenidos/grado07/guion08/Escaleta CN_07_08_CO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\German\Documents\GitHub\CienciasNaturales\fuentes\contenidos\grado07\guion08\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\German\Documents\Aulaplaneta All\Trabajos de editor\EDITOR\ESCALETAS\Escaletas  grupo  3\CN_07_08_CO\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -812,7 +812,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -885,6 +885,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="4">
     <border>
@@ -942,7 +948,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1067,33 +1073,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1136,6 +1115,34 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -1443,8 +1450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:J2"/>
+    <sheetView tabSelected="1" topLeftCell="B22" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="J50" sqref="J50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1474,94 +1481,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="6" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="85" t="s">
+      <c r="A1" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="87" t="s">
+      <c r="B1" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="89" t="s">
+      <c r="C1" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="85" t="s">
+      <c r="D1" s="76" t="s">
         <v>111</v>
       </c>
-      <c r="E1" s="87" t="s">
+      <c r="E1" s="78" t="s">
         <v>112</v>
       </c>
-      <c r="F1" s="91" t="s">
+      <c r="F1" s="82" t="s">
         <v>113</v>
       </c>
-      <c r="G1" s="83" t="s">
+      <c r="G1" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="91" t="s">
+      <c r="H1" s="82" t="s">
         <v>114</v>
       </c>
-      <c r="I1" s="91" t="s">
+      <c r="I1" s="82" t="s">
         <v>108</v>
       </c>
-      <c r="J1" s="93" t="s">
+      <c r="J1" s="84" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="95" t="s">
+      <c r="K1" s="86" t="s">
         <v>109</v>
       </c>
-      <c r="L1" s="83" t="s">
+      <c r="L1" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="78" t="s">
+      <c r="M1" s="92" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="78"/>
-      <c r="O1" s="79" t="s">
+      <c r="N1" s="92"/>
+      <c r="O1" s="93" t="s">
         <v>110</v>
       </c>
-      <c r="P1" s="79" t="s">
+      <c r="P1" s="93" t="s">
         <v>115</v>
       </c>
-      <c r="Q1" s="76" t="s">
+      <c r="Q1" s="90" t="s">
         <v>86</v>
       </c>
-      <c r="R1" s="81" t="s">
+      <c r="R1" s="95" t="s">
         <v>87</v>
       </c>
-      <c r="S1" s="76" t="s">
+      <c r="S1" s="90" t="s">
         <v>88</v>
       </c>
-      <c r="T1" s="74" t="s">
+      <c r="T1" s="88" t="s">
         <v>89</v>
       </c>
-      <c r="U1" s="76" t="s">
+      <c r="U1" s="90" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="6" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="86"/>
-      <c r="B2" s="88"/>
-      <c r="C2" s="90"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="92"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="92"/>
-      <c r="I2" s="92"/>
-      <c r="J2" s="94"/>
-      <c r="K2" s="96"/>
-      <c r="L2" s="84"/>
+      <c r="A2" s="77"/>
+      <c r="B2" s="79"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="83"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="83"/>
+      <c r="I2" s="83"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="87"/>
+      <c r="L2" s="75"/>
       <c r="M2" s="7" t="s">
         <v>91</v>
       </c>
       <c r="N2" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="O2" s="80"/>
-      <c r="P2" s="80"/>
-      <c r="Q2" s="77"/>
-      <c r="R2" s="82"/>
-      <c r="S2" s="77"/>
-      <c r="T2" s="75"/>
-      <c r="U2" s="77"/>
+      <c r="O2" s="94"/>
+      <c r="P2" s="94"/>
+      <c r="Q2" s="91"/>
+      <c r="R2" s="96"/>
+      <c r="S2" s="91"/>
+      <c r="T2" s="89"/>
+      <c r="U2" s="91"/>
     </row>
     <row r="3" spans="1:21" s="31" customFormat="1" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="49" t="s">
@@ -2465,7 +2472,7 @@
       <c r="T22" s="62"/>
       <c r="U22" s="60"/>
     </row>
-    <row r="23" spans="1:21" s="31" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" s="31" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="49" t="s">
         <v>122</v>
       </c>
@@ -2493,7 +2500,7 @@
       <c r="I23" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="J23" s="56" t="s">
+      <c r="J23" s="97" t="s">
         <v>235</v>
       </c>
       <c r="K23" s="57" t="s">
@@ -3251,7 +3258,7 @@
       <c r="I39" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="J39" s="56" t="s">
+      <c r="J39" s="97" t="s">
         <v>204</v>
       </c>
       <c r="K39" s="57" t="s">
@@ -3719,7 +3726,7 @@
       </c>
       <c r="O47" s="42"/>
       <c r="P47" s="55" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q47" s="45">
         <v>6</v>
@@ -4835,6 +4842,14 @@
   </sheetData>
   <autoFilter ref="A2:V47"/>
   <mergeCells count="20">
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="S1:S2"/>
     <mergeCell ref="L1:L2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
@@ -4847,14 +4862,6 @@
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="K1:K2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="O1:O2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="S1:S2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="O23" r:id="rId1"/>

</xml_diff>